<commit_message>
add Hyper connection of report on excel
</commit_message>
<xml_diff>
--- a/Run.xlsx
+++ b/Run.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17070" windowHeight="4965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17070" windowHeight="4965" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestFunction" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,15 @@
     <sheet name="Sanity" sheetId="13" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DNP3'!$B$1:$F$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Modbus!$B$1:$F$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DNP3'!$B$1:$F$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Modbus!$B$1:$F$11</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
   <si>
     <t>TestFunction</t>
   </si>
@@ -154,6 +154,44 @@
   <si>
     <t>192.168.129.49</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestFunction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Src\Output\Run_Test_Case_D1.log</t>
+  </si>
+  <si>
+    <t>Src\Output\Run_Test_Case_D1.log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Src\Output\Run_Test_Case_D2.log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Src\Output\Run_Test_Case_D2.log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Src\Output\Run_Test_Case_D2.log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Src\Output\Run_Test_Case_D3.log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Src\Output\Run_Test_Case_D3.log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Src\Output\Run_FullTest_DNP3.log</t>
   </si>
 </sst>
 </file>
@@ -304,7 +342,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -335,6 +373,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -664,8 +703,8 @@
   <sheetPr codeName="工作表1"/>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -836,10 +875,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="工作表2"/>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD10"/>
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -849,12 +888,12 @@
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>24</v>
@@ -874,135 +913,170 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="12" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="11"/>
+        <v>11</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="11">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="E4" s="8"/>
-      <c r="F4" s="11"/>
+      <c r="F4" s="12" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="11"/>
+        <v>21</v>
+      </c>
+      <c r="D5" s="11">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="12" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="11"/>
+        <v>11</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8"/>
-      <c r="F7" s="11"/>
+      <c r="F7" s="12" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="11"/>
+        <v>33</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="12" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="11">
-        <v>1</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="11">
+        <v>1</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D11" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="11"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:F10"/>
+  <autoFilter ref="B1:F11"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A1" location="TestFunction!A1" display="TestFunction"/>
     <hyperlink ref="A1" location="TestFunction!A1" display="TestFunction"/>
     <hyperlink ref="A1" location="TestFunction!A1" display="TestFunction"/>
     <hyperlink ref="A1" location="TestFunction!A1" display="TestFunction"/>
+    <hyperlink ref="F3:F5" r:id="rId1" display="Src\Output\Run_Test_Case_D1.log"/>
+    <hyperlink ref="F6:F8" r:id="rId2" display="Src\Output\Run_Test_Case_D2.log"/>
+    <hyperlink ref="F2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1010,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1048,30 +1122,26 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="8"/>
+        <v>11</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1079,27 +1149,25 @@
         <v>26</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="11">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>10</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D5" s="11">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1107,12 +1175,14 @@
         <v>27</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="8"/>
+        <v>11</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1120,27 +1190,25 @@
         <v>27</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>10</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E8" s="8"/>
       <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1148,12 +1216,14 @@
         <v>28</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="11">
-        <v>1</v>
-      </c>
-      <c r="E9" s="8"/>
+        <v>9</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1161,16 +1231,29 @@
         <v>28</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>33</v>
+        <v>23</v>
+      </c>
+      <c r="D10" s="11">
+        <v>1</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="11"/>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="11"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:F10"/>
+  <autoFilter ref="B1:F11"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A1" location="TestFunction!A1" display="TestFunction"/>

</xml_diff>

<commit_message>
framework modify from Jamel
</commit_message>
<xml_diff>
--- a/Run.xlsx
+++ b/Run.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17070" windowHeight="4965"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="TestFunction" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DNP3'!$B$1:$F$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Modbus!$B$1:$F$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Modbus!$B$1:$F$12</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="83">
   <si>
     <t>TestFunction</t>
   </si>
@@ -35,306 +35,314 @@
     <t>X</t>
   </si>
   <si>
+    <t>TestResult</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>TestFunction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Masterip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.127.49</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modbus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DNP3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Case_D2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Variable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Case_D1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Channel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Case</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Case_M1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Case_M2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.127.100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.129.49</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestFunction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Src\Output\Run_Test_Case_D1.log</t>
+  </si>
+  <si>
+    <t>Src\Output\Run_Test_Case_D1.log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Src\Output\Run_Test_Case_D2.log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Src\Output\Run_Test_Case_D2.log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Src\Output\Run_Test_Case_D2.log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Src\Output\Run_FullTest_DNP3.log</t>
+  </si>
+  <si>
+    <t>CyberSecurity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TelIP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtIP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pswd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.128.100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aaron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adminmoxa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ips</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eth1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack which IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Telnet IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Telnet Account</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Telnet Pswd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack fron which Interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IpsAttack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DosAttack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TelIP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pswd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IdsFilter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>in_file_dir</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TelIP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pawd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eth1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./../Replay/Rewrite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>path of replay pkt dir</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EDR-G9010</t>
+  </si>
+  <si>
+    <t>IEF</t>
+  </si>
+  <si>
     <t>V</t>
   </si>
   <si>
-    <t>TestResult</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>TestFunction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mip</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Masterip</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.127.49</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Modbus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DNP3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Case_D1</t>
+  </si>
+  <si>
+    <t>Case_D2</t>
   </si>
   <si>
     <t>All</t>
   </si>
   <si>
-    <t>Case_D2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Variable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Case_D1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Case_D3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sip</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sip</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Channel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Address</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Channel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Case</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Address</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Case_M1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Case_M2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Case_M3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Case_D1</t>
-  </si>
-  <si>
-    <t>Case_D2</t>
-  </si>
-  <si>
-    <t>Case_M1</t>
-  </si>
-  <si>
-    <t>192.168.127.49</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.127.100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.129.49</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TestFunction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Src\Output\Run_Test_Case_D1.log</t>
-  </si>
-  <si>
-    <t>Src\Output\Run_Test_Case_D1.log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Src\Output\Run_Test_Case_D2.log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Src\Output\Run_Test_Case_D2.log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Src\Output\Run_Test_Case_D2.log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Src\Output\Run_Test_Case_D3.log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Src\Output\Run_Test_Case_D3.log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>All</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Src\Output\Run_FullTest_DNP3.log</t>
-  </si>
-  <si>
-    <t>CyberSecurity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TelIP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AtIP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pswd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interface</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.128.100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>aaron</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>adminmoxa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ips</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eth1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attack which IP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Telnet IP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Telnet Account</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Telnet Pswd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attack Type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attack fron which Interface</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IpsAttack</t>
-  </si>
-  <si>
-    <t>IpsAttack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IdsFilter</t>
-  </si>
-  <si>
-    <t>DosAttack</t>
-  </si>
-  <si>
-    <t>DosAttack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TelIP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pswd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interface</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IdsFilter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interface</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>in_file_dir</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TelIP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pawd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eth1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>./../Replay/Rewrite</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>path of replay pkt dir</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EDR-G9010</t>
+  </si>
+  <si>
+    <t>Var1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M1-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M1-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M1-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M1-4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M2-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M2-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M2-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DPITest</t>
+  </si>
+  <si>
+    <t>DPITest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -861,7 +869,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -880,31 +888,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>1</v>
@@ -916,39 +924,39 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
-        <v>64</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
@@ -1023,24 +1031,27 @@
       <formula>#REF!="IPSecMaxTunnel"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="6">
+  <dataValidations count="7">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B3:D3">
       <formula1>"V,X"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B4:B10">
       <formula1>"All,Case_D1, Case_D2"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C4:C10">
-      <formula1>"All, Case_M1"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D4:D10">
-      <formula1>"All, IpsAttack, DosAttack, IdsFilter"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:D2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:C2">
       <formula1>"EDR-G9010, EDR-800, EDR-900"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G4 G2">
       <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2">
+      <formula1>"IEF, IEC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C4:C10">
+      <formula1>"All, Case_M1, Case_M2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D4:D10">
+      <formula1>"All, IpsAttack, DosAttack, IdsFilter, DPITest"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -1059,7 +1070,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B9" sqref="B9:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1074,175 +1085,149 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F1" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="10"/>
       <c r="E2" s="7"/>
       <c r="F2" s="11" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="F3" s="11" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="11" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D5" s="10">
         <v>1</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="11" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="F6" s="11" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="11" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="11" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>39</v>
-      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="10">
-        <v>1</v>
-      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="7"/>
-      <c r="F10" s="11" t="s">
-        <v>40</v>
-      </c>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>31</v>
-      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="11" t="s">
-        <v>39</v>
-      </c>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F12" s="11"/>
@@ -1265,9 +1250,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1281,27 +1268,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F1" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="10"/>
@@ -1310,143 +1297,137 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="10">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>8</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E6" s="7"/>
       <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="7"/>
+        <v>78</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>8</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E9" s="7"/>
       <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="10">
-        <v>1</v>
-      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="7"/>
       <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>31</v>
-      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="7"/>
       <c r="F11" s="10"/>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="10"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:F11"/>
+  <autoFilter ref="B1:F12"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A1" location="TestFunction!A1" display="TestFunction"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1461,27 +1442,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F1" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="10"/>
@@ -1490,246 +1471,255 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="10"/>
+        <v>82</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>59</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="7"/>
+        <v>56</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>73</v>
+        <v>50</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>58</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>